<commit_message>
fix(data): Fix data inconsistency
"Toxic_bitmidi" was labelled recognizable, despite having empty labels. This track has been entirely removed for now
</commit_message>
<xml_diff>
--- a/data/song_theme_label_database.xlsx
+++ b/data/song_theme_label_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chuangcaleb/Documents/1Notts/fyp/music-theme-recognition/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BD48B0-1E68-0E40-A0E2-B9E3F5776975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAD7649-FC17-B84E-BFB0-EC07E42FA259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20469,6 +20469,9 @@
       <c r="B544" t="s">
         <v>30</v>
       </c>
+      <c r="D544">
+        <v>0</v>
+      </c>
     </row>
     <row r="545" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A545" t="s">

</xml_diff>